<commit_message>
cross entropy has been added.
</commit_message>
<xml_diff>
--- a/DL_course_plan.xlsx
+++ b/DL_course_plan.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Prath\workspace\AI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA2FFDA6-F08A-4253-8D0A-969BC76D38B9}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33B383C3-4EA3-4226-AFCF-DD7C0322C97B}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8D718CE3-ED35-40C3-943D-443590721FD6}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{8D718CE3-ED35-40C3-943D-443590721FD6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -221,7 +221,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="[h]:mm:ss;@"/>
+    <numFmt numFmtId="164" formatCode="[h]:mm:ss;@"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -275,18 +275,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -603,15 +600,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F286628A-4FB4-47E3-A761-295C51E04924}">
   <dimension ref="A3:F94"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
-      <selection activeCell="C71" sqref="C71"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="12.88671875" customWidth="1"/>
     <col min="2" max="2" width="80.77734375" customWidth="1"/>
-    <col min="3" max="3" width="11.77734375" style="10" customWidth="1"/>
+    <col min="3" max="3" width="11.77734375" style="7" customWidth="1"/>
     <col min="4" max="4" width="12.33203125" customWidth="1"/>
     <col min="5" max="5" width="13.21875" customWidth="1"/>
     <col min="6" max="6" width="14.44140625" customWidth="1"/>
@@ -624,7 +621,7 @@
       <c r="B3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="C3" s="5" t="s">
         <v>1</v>
       </c>
       <c r="D3" s="2" t="s">
@@ -640,11 +637,11 @@
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
       <c r="B4" s="2"/>
-      <c r="C4" s="8">
+      <c r="C4" s="6">
         <v>0.19097222222222221</v>
       </c>
-      <c r="D4" s="5">
-        <v>0.19097222222222221</v>
+      <c r="D4" s="3">
+        <v>9.5833333333333326E-2</v>
       </c>
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
@@ -656,77 +653,77 @@
       <c r="B5" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="7"/>
+      <c r="C5" s="5"/>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="1"/>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="7"/>
+      <c r="C6" s="5"/>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="1"/>
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="7"/>
+      <c r="C7" s="5"/>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="1"/>
-      <c r="B8" s="4" t="s">
+      <c r="B8" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C8" s="7"/>
+      <c r="C8" s="5"/>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="1"/>
-      <c r="B9" s="4" t="s">
+      <c r="B9" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C9" s="7"/>
+      <c r="C9" s="5"/>
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
       <c r="F9" s="2"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="1"/>
-      <c r="B10" s="4" t="s">
+      <c r="B10" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C10" s="7"/>
+      <c r="C10" s="5"/>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="1"/>
-      <c r="B11" s="4" t="s">
+      <c r="B11" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C11" s="7"/>
+      <c r="C11" s="5"/>
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="1"/>
-      <c r="B12" s="4" t="s">
+      <c r="B12" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C12" s="7">
+      <c r="C12" s="5">
         <f>SUM(C4:C11)</f>
         <v>0.19097222222222221</v>
       </c>
@@ -736,8 +733,8 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" s="1"/>
-      <c r="B13" s="4"/>
-      <c r="C13" s="7"/>
+      <c r="B13" s="1"/>
+      <c r="C13" s="5"/>
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
@@ -749,7 +746,7 @@
       <c r="B14" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C14" s="7"/>
+      <c r="C14" s="5"/>
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
@@ -759,7 +756,7 @@
       <c r="B15" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C15" s="9">
+      <c r="C15" s="6">
         <v>0.16666666666666666</v>
       </c>
       <c r="D15" s="3">
@@ -773,7 +770,7 @@
       <c r="B16" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C16" s="9">
+      <c r="C16" s="6">
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="D16" s="1"/>
@@ -785,7 +782,7 @@
       <c r="B17" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C17" s="9">
+      <c r="C17" s="6">
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="D17" s="1"/>
@@ -797,7 +794,7 @@
       <c r="B18" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C18" s="9">
+      <c r="C18" s="6">
         <v>1.3888888888888888E-2</v>
       </c>
       <c r="D18" s="1"/>
@@ -809,14 +806,14 @@
       <c r="B19" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="C19" s="9">
+      <c r="C19" s="6">
         <v>0.33333333333333331</v>
       </c>
       <c r="D19" s="1"/>
       <c r="E19" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F19" s="6">
+      <c r="F19" s="4">
         <v>43522</v>
       </c>
     </row>
@@ -825,7 +822,7 @@
       <c r="B20" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C20" s="9">
+      <c r="C20" s="6">
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="D20" s="1"/>
@@ -837,7 +834,7 @@
       <c r="B21" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C21" s="9">
+      <c r="C21" s="6">
         <v>0.1111111111111111</v>
       </c>
       <c r="D21" s="1"/>
@@ -847,7 +844,7 @@
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
-      <c r="C22" s="7">
+      <c r="C22" s="5">
         <f>SUM(C15:C21)</f>
         <v>0.79166666666666652</v>
       </c>
@@ -862,17 +859,17 @@
       <c r="B23" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C23" s="9"/>
+      <c r="C23" s="6"/>
       <c r="D23" s="1"/>
       <c r="E23" s="1"/>
       <c r="F23" s="1"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" s="1"/>
-      <c r="B24" s="4" t="s">
+      <c r="B24" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C24" s="9">
+      <c r="C24" s="6">
         <v>0.41666666666666669</v>
       </c>
       <c r="D24" s="1"/>
@@ -884,7 +881,7 @@
       <c r="B25" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C25" s="9">
+      <c r="C25" s="6">
         <v>2.7777777777777776E-2</v>
       </c>
       <c r="D25" s="1"/>
@@ -896,7 +893,7 @@
       <c r="B26" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C26" s="9">
+      <c r="C26" s="6">
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="D26" s="1"/>
@@ -908,7 +905,7 @@
       <c r="B27" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C27" s="9">
+      <c r="C27" s="6">
         <v>5.5555555555555552E-2</v>
       </c>
       <c r="D27" s="1"/>
@@ -920,7 +917,7 @@
       <c r="B28" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C28" s="9">
+      <c r="C28" s="6">
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="D28" s="1"/>
@@ -932,7 +929,7 @@
       <c r="B29" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C29" s="9">
+      <c r="C29" s="6">
         <v>0.1388888888888889</v>
       </c>
       <c r="D29" s="1"/>
@@ -944,12 +941,12 @@
       <c r="B30" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C30" s="9">
+      <c r="C30" s="6">
         <v>0.33333333333333331</v>
       </c>
       <c r="D30" s="1"/>
       <c r="E30" s="1"/>
-      <c r="F30" s="6">
+      <c r="F30" s="4">
         <v>43542</v>
       </c>
     </row>
@@ -958,7 +955,7 @@
       <c r="B31" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="C31" s="9">
+      <c r="C31" s="6">
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="D31" s="1"/>
@@ -970,19 +967,19 @@
       <c r="B32" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C32" s="9">
+      <c r="C32" s="6">
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="D32" s="1"/>
       <c r="E32" s="1"/>
-      <c r="F32" s="6">
+      <c r="F32" s="4">
         <v>43542</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" s="1"/>
       <c r="B33" s="1"/>
-      <c r="C33" s="7">
+      <c r="C33" s="5">
         <f>SUM(C24:C32)</f>
         <v>1.2638888888888888</v>
       </c>
@@ -997,17 +994,17 @@
       <c r="B34" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="C34" s="9"/>
+      <c r="C34" s="6"/>
       <c r="D34" s="1"/>
       <c r="E34" s="1"/>
       <c r="F34" s="1"/>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35" s="1"/>
-      <c r="B35" s="4" t="s">
+      <c r="B35" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C35" s="9">
+      <c r="C35" s="6">
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="D35" s="1"/>
@@ -1019,7 +1016,7 @@
       <c r="B36" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C36" s="9">
+      <c r="C36" s="6">
         <v>5.5555555555555552E-2</v>
       </c>
       <c r="D36" s="1"/>
@@ -1031,7 +1028,7 @@
       <c r="B37" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C37" s="9">
+      <c r="C37" s="6">
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="D37" s="1"/>
@@ -1043,7 +1040,7 @@
       <c r="B38" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="C38" s="9">
+      <c r="C38" s="6">
         <v>6.9444444444444434E-2</v>
       </c>
       <c r="D38" s="1"/>
@@ -1055,7 +1052,7 @@
       <c r="B39" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="C39" s="9">
+      <c r="C39" s="6">
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="D39" s="1"/>
@@ -1067,7 +1064,7 @@
       <c r="B40" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C40" s="9">
+      <c r="C40" s="6">
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="D40" s="1"/>
@@ -1079,12 +1076,12 @@
       <c r="B41" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="C41" s="9">
+      <c r="C41" s="6">
         <v>0.33333333333333331</v>
       </c>
       <c r="D41" s="1"/>
       <c r="E41" s="1"/>
-      <c r="F41" s="6">
+      <c r="F41" s="4">
         <v>43573</v>
       </c>
     </row>
@@ -1093,7 +1090,7 @@
       <c r="B42" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="C42" s="9">
+      <c r="C42" s="6">
         <v>7.6388888888888895E-2</v>
       </c>
       <c r="D42" s="1"/>
@@ -1103,7 +1100,7 @@
     <row r="43" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A43" s="1"/>
       <c r="B43" s="1"/>
-      <c r="C43" s="7">
+      <c r="C43" s="5">
         <f>SUM(C35:C42)</f>
         <v>0.86805555555555536</v>
       </c>
@@ -1118,7 +1115,7 @@
       <c r="B44" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="C44" s="9"/>
+      <c r="C44" s="6"/>
       <c r="D44" s="1"/>
       <c r="E44" s="1"/>
       <c r="F44" s="1"/>
@@ -1128,7 +1125,7 @@
       <c r="B45" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="C45" s="9">
+      <c r="C45" s="6">
         <v>0.125</v>
       </c>
       <c r="D45" s="1"/>
@@ -1140,7 +1137,7 @@
       <c r="B46" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="C46" s="9">
+      <c r="C46" s="6">
         <v>0.375</v>
       </c>
       <c r="D46" s="1"/>
@@ -1152,7 +1149,7 @@
       <c r="B47" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="C47" s="9">
+      <c r="C47" s="6">
         <v>0.125</v>
       </c>
       <c r="D47" s="1"/>
@@ -1164,7 +1161,7 @@
       <c r="B48" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="C48" s="9">
+      <c r="C48" s="6">
         <v>0.16666666666666666</v>
       </c>
       <c r="D48" s="1"/>
@@ -1176,19 +1173,19 @@
       <c r="B49" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="C49" s="9">
+      <c r="C49" s="6">
         <v>0.33333333333333331</v>
       </c>
       <c r="D49" s="1"/>
       <c r="E49" s="1"/>
-      <c r="F49" s="6">
+      <c r="F49" s="4">
         <v>43603</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A50" s="1"/>
       <c r="B50" s="1"/>
-      <c r="C50" s="7">
+      <c r="C50" s="5">
         <f>SUM(C45:C49)</f>
         <v>1.125</v>
       </c>
@@ -1203,7 +1200,7 @@
       <c r="B51" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="C51" s="9"/>
+      <c r="C51" s="6"/>
       <c r="D51" s="1"/>
       <c r="E51" s="1"/>
       <c r="F51" s="1"/>
@@ -1213,7 +1210,7 @@
       <c r="B52" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="C52" s="9">
+      <c r="C52" s="6">
         <v>0.1875</v>
       </c>
       <c r="D52" s="1"/>
@@ -1225,7 +1222,7 @@
       <c r="B53" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="C53" s="9">
+      <c r="C53" s="6">
         <v>0.125</v>
       </c>
       <c r="D53" s="1"/>
@@ -1237,7 +1234,7 @@
       <c r="B54" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="C54" s="9">
+      <c r="C54" s="6">
         <v>0.1388888888888889</v>
       </c>
       <c r="D54" s="1"/>
@@ -1249,7 +1246,7 @@
       <c r="B55" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="C55" s="9">
+      <c r="C55" s="6">
         <v>0.125</v>
       </c>
       <c r="D55" s="1"/>
@@ -1261,7 +1258,7 @@
       <c r="B56" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="C56" s="9">
+      <c r="C56" s="6">
         <v>0.1388888888888889</v>
       </c>
       <c r="D56" s="1"/>
@@ -1273,7 +1270,7 @@
       <c r="B57" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="C57" s="7">
+      <c r="C57" s="5">
         <f>SUM(C52:C56)</f>
         <v>0.71527777777777768</v>
       </c>
@@ -1284,7 +1281,7 @@
     <row r="58" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A58" s="1"/>
       <c r="B58" s="1"/>
-      <c r="C58" s="9"/>
+      <c r="C58" s="6"/>
       <c r="D58" s="1"/>
       <c r="E58" s="1"/>
       <c r="F58" s="1"/>
@@ -1296,7 +1293,7 @@
       <c r="B59" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="C59" s="9"/>
+      <c r="C59" s="6"/>
       <c r="D59" s="1"/>
       <c r="E59" s="1"/>
       <c r="F59" s="1"/>
@@ -1306,7 +1303,7 @@
       <c r="B60" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="C60" s="9">
+      <c r="C60" s="6">
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="D60" s="1"/>
@@ -1318,7 +1315,7 @@
       <c r="B61" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="C61" s="9">
+      <c r="C61" s="6">
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="D61" s="1"/>
@@ -1330,7 +1327,7 @@
       <c r="B62" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="C62" s="9">
+      <c r="C62" s="6">
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="D62" s="1"/>
@@ -1340,7 +1337,7 @@
     <row r="63" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A63" s="1"/>
       <c r="B63" s="1"/>
-      <c r="C63" s="7">
+      <c r="C63" s="5">
         <f>SUM(C60:C62)</f>
         <v>0.16666666666666666</v>
       </c>
@@ -1355,7 +1352,7 @@
       <c r="B64" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="C64" s="9"/>
+      <c r="C64" s="6"/>
       <c r="D64" s="1"/>
       <c r="E64" s="1"/>
       <c r="F64" s="1"/>
@@ -1365,7 +1362,7 @@
       <c r="B65" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="C65" s="9">
+      <c r="C65" s="6">
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="D65" s="1"/>
@@ -1377,7 +1374,7 @@
       <c r="B66" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="C66" s="9">
+      <c r="C66" s="6">
         <v>6.9444444444444434E-2</v>
       </c>
       <c r="D66" s="1"/>
@@ -1389,7 +1386,7 @@
       <c r="B67" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="C67" s="9">
+      <c r="C67" s="6">
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="D67" s="1"/>
@@ -1399,7 +1396,7 @@
     <row r="68" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A68" s="1"/>
       <c r="B68" s="1"/>
-      <c r="C68" s="9">
+      <c r="C68" s="6">
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="D68" s="1"/>
@@ -1409,7 +1406,7 @@
     <row r="69" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A69" s="1"/>
       <c r="B69" s="1"/>
-      <c r="C69" s="7">
+      <c r="C69" s="5">
         <f>SUM(C65:C68)</f>
         <v>0.27777777777777773</v>
       </c>
@@ -1420,7 +1417,7 @@
     <row r="70" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A70" s="1"/>
       <c r="B70" s="1"/>
-      <c r="C70" s="9"/>
+      <c r="C70" s="6"/>
       <c r="D70" s="1"/>
       <c r="E70" s="1"/>
       <c r="F70" s="1"/>
@@ -1430,7 +1427,7 @@
       <c r="B71" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="C71" s="7">
+      <c r="C71" s="5">
         <f>SUM(C12,C22,C33,C43,C50,C57,C63,C69)</f>
         <v>5.3993055555555554</v>
       </c>
@@ -1441,7 +1438,7 @@
     <row r="72" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A72" s="1"/>
       <c r="B72" s="1"/>
-      <c r="C72" s="9"/>
+      <c r="C72" s="6"/>
       <c r="D72" s="1"/>
       <c r="E72" s="1"/>
       <c r="F72" s="1"/>
@@ -1449,7 +1446,7 @@
     <row r="73" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A73" s="1"/>
       <c r="B73" s="1"/>
-      <c r="C73" s="9"/>
+      <c r="C73" s="6"/>
       <c r="D73" s="1"/>
       <c r="E73" s="1"/>
       <c r="F73" s="1"/>
@@ -1457,7 +1454,7 @@
     <row r="74" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A74" s="1"/>
       <c r="B74" s="1"/>
-      <c r="C74" s="9"/>
+      <c r="C74" s="6"/>
       <c r="D74" s="1"/>
       <c r="E74" s="1"/>
       <c r="F74" s="1"/>
@@ -1465,7 +1462,7 @@
     <row r="75" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A75" s="1"/>
       <c r="B75" s="1"/>
-      <c r="C75" s="9"/>
+      <c r="C75" s="6"/>
       <c r="D75" s="1"/>
       <c r="E75" s="1"/>
       <c r="F75" s="1"/>
@@ -1473,7 +1470,7 @@
     <row r="76" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A76" s="1"/>
       <c r="B76" s="1"/>
-      <c r="C76" s="9"/>
+      <c r="C76" s="6"/>
       <c r="D76" s="1"/>
       <c r="E76" s="1"/>
       <c r="F76" s="1"/>
@@ -1481,7 +1478,7 @@
     <row r="77" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A77" s="1"/>
       <c r="B77" s="1"/>
-      <c r="C77" s="9"/>
+      <c r="C77" s="6"/>
       <c r="D77" s="1"/>
       <c r="E77" s="1"/>
       <c r="F77" s="1"/>
@@ -1489,7 +1486,7 @@
     <row r="78" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A78" s="1"/>
       <c r="B78" s="1"/>
-      <c r="C78" s="9"/>
+      <c r="C78" s="6"/>
       <c r="D78" s="1"/>
       <c r="E78" s="1"/>
       <c r="F78" s="1"/>
@@ -1497,7 +1494,7 @@
     <row r="79" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A79" s="1"/>
       <c r="B79" s="1"/>
-      <c r="C79" s="9"/>
+      <c r="C79" s="6"/>
       <c r="D79" s="1"/>
       <c r="E79" s="1"/>
       <c r="F79" s="1"/>
@@ -1505,7 +1502,7 @@
     <row r="80" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A80" s="1"/>
       <c r="B80" s="1"/>
-      <c r="C80" s="9"/>
+      <c r="C80" s="6"/>
       <c r="D80" s="1"/>
       <c r="E80" s="1"/>
       <c r="F80" s="1"/>
@@ -1513,7 +1510,7 @@
     <row r="81" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A81" s="1"/>
       <c r="B81" s="1"/>
-      <c r="C81" s="9"/>
+      <c r="C81" s="6"/>
       <c r="D81" s="1"/>
       <c r="E81" s="1"/>
       <c r="F81" s="1"/>
@@ -1521,7 +1518,7 @@
     <row r="82" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A82" s="1"/>
       <c r="B82" s="1"/>
-      <c r="C82" s="9"/>
+      <c r="C82" s="6"/>
       <c r="D82" s="1"/>
       <c r="E82" s="1"/>
       <c r="F82" s="1"/>
@@ -1529,7 +1526,7 @@
     <row r="83" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A83" s="1"/>
       <c r="B83" s="1"/>
-      <c r="C83" s="9"/>
+      <c r="C83" s="6"/>
       <c r="D83" s="1"/>
       <c r="E83" s="1"/>
       <c r="F83" s="1"/>
@@ -1537,7 +1534,7 @@
     <row r="84" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A84" s="1"/>
       <c r="B84" s="1"/>
-      <c r="C84" s="9"/>
+      <c r="C84" s="6"/>
       <c r="D84" s="1"/>
       <c r="E84" s="1"/>
       <c r="F84" s="1"/>
@@ -1545,7 +1542,7 @@
     <row r="85" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A85" s="1"/>
       <c r="B85" s="1"/>
-      <c r="C85" s="9"/>
+      <c r="C85" s="6"/>
       <c r="D85" s="1"/>
       <c r="E85" s="1"/>
       <c r="F85" s="1"/>
@@ -1553,7 +1550,7 @@
     <row r="86" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A86" s="1"/>
       <c r="B86" s="1"/>
-      <c r="C86" s="9"/>
+      <c r="C86" s="6"/>
       <c r="D86" s="1"/>
       <c r="E86" s="1"/>
       <c r="F86" s="1"/>
@@ -1561,7 +1558,7 @@
     <row r="87" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A87" s="1"/>
       <c r="B87" s="1"/>
-      <c r="C87" s="9"/>
+      <c r="C87" s="6"/>
       <c r="D87" s="1"/>
       <c r="E87" s="1"/>
       <c r="F87" s="1"/>
@@ -1569,7 +1566,7 @@
     <row r="88" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A88" s="1"/>
       <c r="B88" s="1"/>
-      <c r="C88" s="9"/>
+      <c r="C88" s="6"/>
       <c r="D88" s="1"/>
       <c r="E88" s="1"/>
       <c r="F88" s="1"/>
@@ -1577,7 +1574,7 @@
     <row r="89" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A89" s="1"/>
       <c r="B89" s="1"/>
-      <c r="C89" s="9"/>
+      <c r="C89" s="6"/>
       <c r="D89" s="1"/>
       <c r="E89" s="1"/>
       <c r="F89" s="1"/>
@@ -1585,7 +1582,7 @@
     <row r="90" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A90" s="1"/>
       <c r="B90" s="1"/>
-      <c r="C90" s="9"/>
+      <c r="C90" s="6"/>
       <c r="D90" s="1"/>
       <c r="E90" s="1"/>
       <c r="F90" s="1"/>
@@ -1593,7 +1590,7 @@
     <row r="91" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A91" s="1"/>
       <c r="B91" s="1"/>
-      <c r="C91" s="9"/>
+      <c r="C91" s="6"/>
       <c r="D91" s="1"/>
       <c r="E91" s="1"/>
       <c r="F91" s="1"/>
@@ -1601,7 +1598,7 @@
     <row r="92" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A92" s="1"/>
       <c r="B92" s="1"/>
-      <c r="C92" s="9"/>
+      <c r="C92" s="6"/>
       <c r="D92" s="1"/>
       <c r="E92" s="1"/>
       <c r="F92" s="1"/>
@@ -1609,7 +1606,7 @@
     <row r="93" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A93" s="1"/>
       <c r="B93" s="1"/>
-      <c r="C93" s="9"/>
+      <c r="C93" s="6"/>
       <c r="D93" s="1"/>
       <c r="E93" s="1"/>
       <c r="F93" s="1"/>
@@ -1617,7 +1614,7 @@
     <row r="94" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A94" s="1"/>
       <c r="B94" s="1"/>
-      <c r="C94" s="9"/>
+      <c r="C94" s="6"/>
       <c r="D94" s="1"/>
       <c r="E94" s="1"/>
       <c r="F94" s="1"/>

</xml_diff>